<commit_message>
Add language bar to home. Handle 500 errors
</commit_message>
<xml_diff>
--- a/KFLA/Data/data.cn.xlsx
+++ b/KFLA/Data/data.cn.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="38 competency questions_Chinese" sheetId="11" r:id="rId1"/>
@@ -27,11 +27,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -51,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="543">
   <si>
     <t>Competency Name</t>
   </si>
@@ -563,93 +558,48 @@
     <t>Stoppers.Loading</t>
   </si>
   <si>
-    <t>Loading stoppers...</t>
-  </si>
-  <si>
     <t>PageTitles.LIBRARY</t>
   </si>
   <si>
-    <t>Competency Library</t>
-  </si>
-  <si>
     <t>PageTitles.COMPETENCIES</t>
   </si>
   <si>
-    <t>Competency Assessment</t>
-  </si>
-  <si>
     <t>PageTitles.QUESTIONS</t>
   </si>
   <si>
-    <t>Behavior-Based Questions</t>
-  </si>
-  <si>
     <t>Home.Title</t>
   </si>
   <si>
-    <t>Korn Ferry Leadership Architectâ„¢</t>
-  </si>
-  <si>
     <t>Home.Internal</t>
   </si>
   <si>
-    <t>For internal use only</t>
-  </si>
-  <si>
     <t>QuestionsResult.Questions</t>
   </si>
   <si>
-    <t>QUESTIONS</t>
-  </si>
-  <si>
     <t>QuestionsResult.Notes</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>QuestionsResult.Empty</t>
   </si>
   <si>
-    <t>No competencies or stoppers selected. Redirrecting...</t>
-  </si>
-  <si>
     <t>Buttons.Print</t>
   </si>
   <si>
-    <t>Print</t>
-  </si>
-  <si>
     <t>Buttons.Info</t>
   </si>
   <si>
-    <t>Info</t>
-  </si>
-  <si>
     <t>Buttons.Submit</t>
   </si>
   <si>
-    <t>Submit</t>
-  </si>
-  <si>
     <t>Buttons.Reset</t>
   </si>
   <si>
-    <t>Reset</t>
-  </si>
-  <si>
     <t>Buttons.Close</t>
   </si>
   <si>
-    <t>Close</t>
-  </si>
-  <si>
     <t>Questionaire.Reset</t>
   </si>
   <si>
-    <t>Are you sure you wish to reset questionaire?</t>
-  </si>
-  <si>
     <t>Questionaire.PasswordRequired</t>
   </si>
   <si>
@@ -677,9 +627,6 @@
     <t>Questionaire.Loading</t>
   </si>
   <si>
-    <t>Loading competencies...</t>
-  </si>
-  <si>
     <t>StopperItem.Problem</t>
   </si>
   <si>
@@ -692,15 +639,9 @@
     <t>Library.SortByNumber</t>
   </si>
   <si>
-    <t>Sort by Competency number</t>
-  </si>
-  <si>
     <t>Library.SortByFactors</t>
   </si>
   <si>
-    <t>Sort by Factors and Clusters</t>
-  </si>
-  <si>
     <t>Skills.SKILLED</t>
   </si>
   <si>
@@ -716,36 +657,21 @@
     <t>RightsReserved</t>
   </si>
   <si>
-    <t>Â© Korn Ferry 2014-2015. All rights reserved.</t>
-  </si>
-  <si>
     <t>Evaluation.Reset</t>
   </si>
   <si>
-    <t>Are you sure you wish to reset evaluation?</t>
-  </si>
-  <si>
     <t>Evaluation.Loading</t>
   </si>
   <si>
     <t>CompetencyItem.Cards</t>
   </si>
   <si>
-    <t>Korn Ferry Leadership Architectâ„¢ Global Competency Framework Sort Cards</t>
-  </si>
-  <si>
     <t>EvaluationResult.Legend</t>
   </si>
   <si>
-    <t>Legend</t>
-  </si>
-  <si>
     <t>EvaluationResult.Empty</t>
   </si>
   <si>
-    <t>No competencies evaluated. Redirrecting...</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -753,15 +679,6 @@
   </si>
   <si>
     <t>Icon</t>
-  </si>
-  <si>
-    <t>Would describe</t>
-  </si>
-  <si>
-    <t>Might describe</t>
-  </si>
-  <si>
-    <t>Would Not describe</t>
   </si>
   <si>
     <t>#007e3a</t>
@@ -2213,6 +2130,102 @@
   </si>
   <si>
     <t xml:space="preserve">Not A Problem </t>
+  </si>
+  <si>
+    <t>阻碍因素载入中…</t>
+  </si>
+  <si>
+    <t>能力文库</t>
+  </si>
+  <si>
+    <t>能力评估</t>
+  </si>
+  <si>
+    <t>行为面试问题</t>
+  </si>
+  <si>
+    <t>仅限于内部使用</t>
+  </si>
+  <si>
+    <t>问题</t>
+  </si>
+  <si>
+    <t>注释</t>
+  </si>
+  <si>
+    <t>未选择能力或阻碍因素。重新选择…</t>
+  </si>
+  <si>
+    <t>打印</t>
+  </si>
+  <si>
+    <t>信息</t>
+  </si>
+  <si>
+    <t>提交</t>
+  </si>
+  <si>
+    <t>重置</t>
+  </si>
+  <si>
+    <t>关闭</t>
+  </si>
+  <si>
+    <t>您确认要重置问卷吗？</t>
+  </si>
+  <si>
+    <t>载入能力…</t>
+  </si>
+  <si>
+    <t>能力编号索引</t>
+  </si>
+  <si>
+    <t>因素和群组索引</t>
+  </si>
+  <si>
+    <t>您确认要重置评估吗？</t>
+  </si>
+  <si>
+    <t>分类说明</t>
+  </si>
+  <si>
+    <t>未进行能力评估。重新选择…</t>
+  </si>
+  <si>
+    <t>高/完全能描述</t>
+  </si>
+  <si>
+    <t>中等/可以描述</t>
+  </si>
+  <si>
+    <t>低/不能描述</t>
+  </si>
+  <si>
+    <t>全部或大多数时候符合</t>
+  </si>
+  <si>
+    <t>有些时候符合，或介于符合与不符合之间</t>
+  </si>
+  <si>
+    <t>基本或很少符合</t>
+  </si>
+  <si>
+    <t>© Korn Ferry 2014-2015. All rights reserved.</t>
+  </si>
+  <si>
+    <t>Korn Ferry Leadership Architect ©Global Competency Framework Sort Cards</t>
+  </si>
+  <si>
+    <t>高或完全能描述</t>
+  </si>
+  <si>
+    <t>中等或可以描述</t>
+  </si>
+  <si>
+    <t>低或不能描述</t>
+  </si>
+  <si>
+    <t>Korn Ferry Leadership Architect</t>
   </si>
 </sst>
 </file>
@@ -2357,7 +2370,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2444,6 +2457,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="columnHeader" xfId="1"/>
@@ -2770,7 +2798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2793,25 +2821,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>526</v>
+        <v>500</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>527</v>
+        <v>501</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>528</v>
+        <v>502</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>529</v>
+        <v>503</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>530</v>
+        <v>504</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>531</v>
+        <v>505</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>532</v>
+        <v>506</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>2</v>
@@ -2831,28 +2859,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>298</v>
+        <v>272</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>336</v>
+        <v>310</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>374</v>
+        <v>348</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>412</v>
+        <v>386</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>450</v>
+        <v>424</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>44</v>
@@ -2870,28 +2898,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>337</v>
+        <v>311</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>375</v>
+        <v>349</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>413</v>
+        <v>387</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>451</v>
+        <v>425</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>47</v>
@@ -2909,28 +2937,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>338</v>
+        <v>312</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>376</v>
+        <v>350</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>414</v>
+        <v>388</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>452</v>
+        <v>426</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>50</v>
@@ -2948,28 +2976,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>339</v>
+        <v>313</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>377</v>
+        <v>351</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>415</v>
+        <v>389</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>453</v>
+        <v>427</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>53</v>
@@ -2989,28 +3017,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>302</v>
+        <v>276</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>378</v>
+        <v>352</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>416</v>
+        <v>390</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>454</v>
+        <v>428</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>55</v>
@@ -3028,28 +3056,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>303</v>
+        <v>277</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>341</v>
+        <v>315</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>379</v>
+        <v>353</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>417</v>
+        <v>391</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>455</v>
+        <v>429</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>5</v>
@@ -3067,28 +3095,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>304</v>
+        <v>278</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>342</v>
+        <v>316</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>380</v>
+        <v>354</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>418</v>
+        <v>392</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>456</v>
+        <v>430</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>60</v>
@@ -3108,28 +3136,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>305</v>
+        <v>279</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>343</v>
+        <v>317</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>381</v>
+        <v>355</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>419</v>
+        <v>393</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>457</v>
+        <v>431</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>64</v>
@@ -3147,28 +3175,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>306</v>
+        <v>280</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>344</v>
+        <v>318</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>382</v>
+        <v>356</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>420</v>
+        <v>394</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>458</v>
+        <v>432</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>67</v>
@@ -3186,28 +3214,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>307</v>
+        <v>281</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>345</v>
+        <v>319</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>383</v>
+        <v>357</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>421</v>
+        <v>395</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>459</v>
+        <v>433</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>70</v>
@@ -3225,28 +3253,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>384</v>
+        <v>358</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>422</v>
+        <v>396</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>460</v>
+        <v>434</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>72</v>
@@ -3266,28 +3294,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>271</v>
+        <v>245</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>309</v>
+        <v>283</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>347</v>
+        <v>321</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>385</v>
+        <v>359</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>423</v>
+        <v>397</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>461</v>
+        <v>435</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>76</v>
@@ -3305,28 +3333,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>348</v>
+        <v>322</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>386</v>
+        <v>360</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>424</v>
+        <v>398</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>462</v>
+        <v>436</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>79</v>
@@ -3346,28 +3374,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>311</v>
+        <v>285</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>387</v>
+        <v>361</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>425</v>
+        <v>399</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>463</v>
+        <v>437</v>
       </c>
       <c r="J15" s="27" t="s">
         <v>83</v>
@@ -3385,28 +3413,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>312</v>
+        <v>286</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>388</v>
+        <v>362</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>426</v>
+        <v>400</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>464</v>
+        <v>438</v>
       </c>
       <c r="J16" s="27" t="s">
         <v>86</v>
@@ -3426,28 +3454,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>313</v>
+        <v>287</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>389</v>
+        <v>363</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>427</v>
+        <v>401</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>465</v>
+        <v>439</v>
       </c>
       <c r="J17" s="27" t="s">
         <v>90</v>
@@ -3465,28 +3493,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>314</v>
+        <v>288</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>352</v>
+        <v>326</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>428</v>
+        <v>402</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>466</v>
+        <v>440</v>
       </c>
       <c r="J18" s="27" t="s">
         <v>93</v>
@@ -3504,28 +3532,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>315</v>
+        <v>289</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>391</v>
+        <v>365</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>429</v>
+        <v>403</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>467</v>
+        <v>441</v>
       </c>
       <c r="J19" s="27" t="s">
         <v>96</v>
@@ -3543,28 +3571,28 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>354</v>
+        <v>328</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>392</v>
+        <v>366</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>430</v>
+        <v>404</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>468</v>
+        <v>442</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>99</v>
@@ -3584,28 +3612,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>279</v>
+        <v>253</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>317</v>
+        <v>291</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>393</v>
+        <v>367</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>431</v>
+        <v>405</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>11</v>
@@ -3623,28 +3651,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>280</v>
+        <v>254</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>356</v>
+        <v>330</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>394</v>
+        <v>368</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>432</v>
+        <v>406</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>470</v>
+        <v>444</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>104</v>
@@ -3662,28 +3690,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>357</v>
+        <v>331</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>395</v>
+        <v>369</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>433</v>
+        <v>407</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>471</v>
+        <v>445</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>107</v>
@@ -3701,28 +3729,28 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>282</v>
+        <v>256</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>320</v>
+        <v>294</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>396</v>
+        <v>370</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>434</v>
+        <v>408</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>472</v>
+        <v>446</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>110</v>
@@ -3740,28 +3768,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>321</v>
+        <v>295</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>397</v>
+        <v>371</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>435</v>
+        <v>409</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>473</v>
+        <v>447</v>
       </c>
       <c r="J25" s="7" t="s">
         <v>113</v>
@@ -3781,28 +3809,28 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>322</v>
+        <v>296</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>360</v>
+        <v>334</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>398</v>
+        <v>372</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>436</v>
+        <v>410</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>474</v>
+        <v>448</v>
       </c>
       <c r="J26" s="7" t="s">
         <v>117</v>
@@ -3822,28 +3850,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>323</v>
+        <v>297</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>399</v>
+        <v>373</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>437</v>
+        <v>411</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>475</v>
+        <v>449</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>121</v>
@@ -3861,28 +3889,28 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>324</v>
+        <v>298</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>362</v>
+        <v>336</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>400</v>
+        <v>374</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>438</v>
+        <v>412</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>124</v>
@@ -3900,28 +3928,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>325</v>
+        <v>299</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>363</v>
+        <v>337</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>401</v>
+        <v>375</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>439</v>
+        <v>413</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>477</v>
+        <v>451</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>127</v>
@@ -3939,28 +3967,28 @@
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>326</v>
+        <v>300</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>402</v>
+        <v>376</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>440</v>
+        <v>414</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>478</v>
+        <v>452</v>
       </c>
       <c r="J30" s="16" t="s">
         <v>130</v>
@@ -3978,28 +4006,28 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>327</v>
+        <v>301</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>365</v>
+        <v>339</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>403</v>
+        <v>377</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>441</v>
+        <v>415</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>479</v>
+        <v>453</v>
       </c>
       <c r="J31" s="7" t="s">
         <v>133</v>
@@ -4017,28 +4045,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>328</v>
+        <v>302</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>366</v>
+        <v>340</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>404</v>
+        <v>378</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>442</v>
+        <v>416</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>480</v>
+        <v>454</v>
       </c>
       <c r="J32" s="16" t="s">
         <v>136</v>
@@ -4056,28 +4084,28 @@
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>329</v>
+        <v>303</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>405</v>
+        <v>379</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>443</v>
+        <v>417</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
       <c r="J33" s="16" t="s">
         <v>139</v>
@@ -4095,28 +4123,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>368</v>
+        <v>342</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>406</v>
+        <v>380</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>444</v>
+        <v>418</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="J34" s="30" t="s">
         <v>142</v>
@@ -4134,28 +4162,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>369</v>
+        <v>343</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>407</v>
+        <v>381</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>445</v>
+        <v>419</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>483</v>
+        <v>457</v>
       </c>
       <c r="J35" s="30" t="s">
         <v>144</v>
@@ -4173,28 +4201,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>332</v>
+        <v>306</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>370</v>
+        <v>344</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>408</v>
+        <v>382</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>446</v>
+        <v>420</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>484</v>
+        <v>458</v>
       </c>
       <c r="J36" s="30" t="s">
         <v>147</v>
@@ -4212,28 +4240,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>333</v>
+        <v>307</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>409</v>
+        <v>383</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>447</v>
+        <v>421</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="J37" s="7" t="s">
         <v>150</v>
@@ -4251,28 +4279,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>296</v>
+        <v>270</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>334</v>
+        <v>308</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>372</v>
+        <v>346</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>410</v>
+        <v>384</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>448</v>
+        <v>422</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="J38" s="7" t="s">
         <v>153</v>
@@ -4290,28 +4318,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>297</v>
+        <v>271</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>373</v>
+        <v>347</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>411</v>
+        <v>385</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>449</v>
+        <v>423</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>487</v>
+        <v>461</v>
       </c>
       <c r="J39" s="7" t="s">
         <v>156</v>
@@ -4358,16 +4386,16 @@
         <v>13</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>533</v>
+        <v>507</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>534</v>
+        <v>508</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>535</v>
+        <v>509</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>536</v>
+        <v>510</v>
       </c>
       <c r="F1" s="23" t="s">
         <v>15</v>
@@ -4387,16 +4415,16 @@
         <v>101</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>488</v>
+        <v>462</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>498</v>
+        <v>472</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>508</v>
+        <v>482</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>19</v>
@@ -4416,16 +4444,16 @@
         <v>102</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>489</v>
+        <v>463</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>499</v>
+        <v>473</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>509</v>
+        <v>483</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>23</v>
@@ -4443,16 +4471,16 @@
         <v>103</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>490</v>
+        <v>464</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>500</v>
+        <v>474</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>510</v>
+        <v>484</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>26</v>
@@ -4468,16 +4496,16 @@
         <v>104</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>491</v>
+        <v>465</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>501</v>
+        <v>475</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>511</v>
+        <v>485</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>28</v>
@@ -4497,16 +4525,16 @@
         <v>105</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>492</v>
+        <v>466</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>502</v>
+        <v>476</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>512</v>
+        <v>486</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>32</v>
@@ -4524,16 +4552,16 @@
         <v>106</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>493</v>
+        <v>467</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>503</v>
+        <v>477</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>513</v>
+        <v>487</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>35</v>
@@ -4547,16 +4575,16 @@
         <v>107</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>494</v>
+        <v>468</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>504</v>
+        <v>478</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>514</v>
+        <v>488</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>36</v>
@@ -4572,16 +4600,16 @@
         <v>108</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>495</v>
+        <v>469</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>505</v>
+        <v>479</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>515</v>
+        <v>489</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>38</v>
@@ -4599,16 +4627,16 @@
         <v>109</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>496</v>
+        <v>470</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>506</v>
+        <v>480</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>516</v>
+        <v>490</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>41</v>
@@ -4622,16 +4650,16 @@
         <v>110</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>497</v>
+        <v>471</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>507</v>
+        <v>481</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>517</v>
+        <v>491</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>42</v>
@@ -4653,8 +4681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4675,336 +4703,336 @@
       <c r="A2" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>524</v>
+      <c r="B2" s="34" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>163</v>
+      <c r="B3" s="34" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>165</v>
+        <v>163</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>167</v>
+        <v>164</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>169</v>
+        <v>165</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>171</v>
+        <v>542</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>173</v>
+        <v>167</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>175</v>
+        <v>168</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>177</v>
+        <v>169</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>179</v>
+        <v>170</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>181</v>
+        <v>171</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>182</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>183</v>
+        <v>172</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
-        <v>184</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>185</v>
+        <v>173</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>187</v>
+        <v>174</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>189</v>
+        <v>175</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>191</v>
+        <v>176</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>201</v>
+        <v>185</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
-        <v>202</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>522</v>
+        <v>186</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="24" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>523</v>
+        <v>187</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>201</v>
+        <v>188</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="26" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>206</v>
+        <v>189</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>207</v>
-      </c>
-      <c r="B27" s="32" t="s">
-        <v>208</v>
+        <v>190</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
-        <v>209</v>
-      </c>
-      <c r="B28" s="32" t="s">
-        <v>519</v>
+        <v>191</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
-        <v>210</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>518</v>
+        <v>192</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>520</v>
+        <v>193</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
-        <v>212</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>521</v>
+        <v>194</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>214</v>
+        <v>537</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
-        <v>215</v>
-      </c>
-      <c r="B33" s="32" t="s">
-        <v>216</v>
+        <v>196</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>217</v>
-      </c>
-      <c r="B34" s="32" t="s">
-        <v>201</v>
+        <v>197</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>219</v>
+        <v>538</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>221</v>
+        <v>199</v>
+      </c>
+      <c r="B36" s="38" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>223</v>
+        <v>200</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
-        <v>525</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>227</v>
+        <v>499</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
-        <v>525</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>228</v>
+        <v>499</v>
+      </c>
+      <c r="B39" s="38" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>525</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>229</v>
+        <v>499</v>
+      </c>
+      <c r="B40" s="38" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
-        <v>525</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>236</v>
+        <v>499</v>
+      </c>
+      <c r="B41" s="38" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
-        <v>525</v>
-      </c>
-      <c r="B42" s="32" t="s">
-        <v>237</v>
+        <v>499</v>
+      </c>
+      <c r="B42" s="38" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>525</v>
-      </c>
-      <c r="B43" s="32" t="s">
-        <v>238</v>
+        <v>499</v>
+      </c>
+      <c r="B43" s="38" t="s">
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -5019,7 +5047,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5034,85 +5062,86 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
       <c r="D1" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="E1" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="F1" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>227</v>
+      <c r="B2" s="21" t="s">
+        <v>539</v>
       </c>
       <c r="C2">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="E2" t="s">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="F2" t="s">
-        <v>236</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>228</v>
+      <c r="B3" s="21" t="s">
+        <v>540</v>
       </c>
       <c r="C3">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="E3" t="s">
-        <v>234</v>
+        <v>208</v>
       </c>
       <c r="F3" t="s">
-        <v>237</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>229</v>
+      <c r="B4" s="21" t="s">
+        <v>541</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
       <c r="E4" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="F4" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix printing of legend.
</commit_message>
<xml_diff>
--- a/KFLA/Data/data.cn.xlsx
+++ b/KFLA/Data/data.cn.xlsx
@@ -22,6 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Stallers and Stoppers_Chinese'!$A$1:$E$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Strings!$A$1:$B$1</definedName>
     <definedName name="list" localSheetId="2">Strings!$A$2:$B$37</definedName>
+    <definedName name="list_1" localSheetId="2">Strings!$A$2:$B$38</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,11 +43,19 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="list1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="E:\Desktop\list.csv" decimal="," thousands=" " tab="0" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="538">
   <si>
     <t>Competency Name</t>
   </si>
@@ -699,15 +708,6 @@
     <t>minus-circle</t>
   </si>
   <si>
-    <t>This would be true all or the majority of the time</t>
-  </si>
-  <si>
-    <t>This would be true some of the time or may be a mixture of would and would not describe</t>
-  </si>
-  <si>
-    <t>This would be seldom or never true</t>
-  </si>
-  <si>
     <t>Limit</t>
   </si>
   <si>
@@ -2096,9 +2096,6 @@
     <t>职业延滞和阻碍因素</t>
   </si>
   <si>
-    <t>Evaluations</t>
-  </si>
-  <si>
     <t xml:space="preserve">Competency Definition </t>
   </si>
   <si>
@@ -2192,15 +2189,6 @@
     <t>未进行能力评估。重新选择…</t>
   </si>
   <si>
-    <t>高/完全能描述</t>
-  </si>
-  <si>
-    <t>中等/可以描述</t>
-  </si>
-  <si>
-    <t>低/不能描述</t>
-  </si>
-  <si>
     <t>全部或大多数时候符合</t>
   </si>
   <si>
@@ -2226,6 +2214,12 @@
   </si>
   <si>
     <t>Korn Ferry Leadership Architect</t>
+  </si>
+  <si>
+    <t>PageTitles.HOME</t>
+  </si>
+  <si>
+    <t>Home</t>
   </si>
 </sst>
 </file>
@@ -2370,7 +2364,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2453,22 +2447,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2496,6 +2475,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="list_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="list" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -2821,25 +2804,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>500</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="H1" s="14" t="s">
         <v>501</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="I1" s="14" t="s">
         <v>502</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>503</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>504</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>505</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>506</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>2</v>
@@ -2859,28 +2842,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>44</v>
@@ -2898,28 +2881,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>47</v>
@@ -2937,28 +2920,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>50</v>
@@ -2976,28 +2959,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>53</v>
@@ -3017,28 +3000,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>55</v>
@@ -3056,28 +3039,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>5</v>
@@ -3095,28 +3078,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>60</v>
@@ -3136,28 +3119,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>64</v>
@@ -3175,28 +3158,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>67</v>
@@ -3214,28 +3197,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>70</v>
@@ -3253,28 +3236,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>72</v>
@@ -3294,28 +3277,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>76</v>
@@ -3333,28 +3316,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>79</v>
@@ -3374,28 +3357,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="J15" s="27" t="s">
         <v>83</v>
@@ -3413,28 +3396,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="J16" s="27" t="s">
         <v>86</v>
@@ -3454,28 +3437,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="J17" s="27" t="s">
         <v>90</v>
@@ -3493,28 +3476,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="J18" s="27" t="s">
         <v>93</v>
@@ -3532,28 +3515,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="J19" s="27" t="s">
         <v>96</v>
@@ -3571,28 +3554,28 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>99</v>
@@ -3612,28 +3595,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>11</v>
@@ -3651,28 +3634,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>104</v>
@@ -3690,28 +3673,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>107</v>
@@ -3729,28 +3712,28 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>110</v>
@@ -3768,28 +3751,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="J25" s="7" t="s">
         <v>113</v>
@@ -3809,28 +3792,28 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="J26" s="7" t="s">
         <v>117</v>
@@ -3850,28 +3833,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>121</v>
@@ -3889,28 +3872,28 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>124</v>
@@ -3928,28 +3911,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>127</v>
@@ -3967,28 +3950,28 @@
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="J30" s="16" t="s">
         <v>130</v>
@@ -4006,28 +3989,28 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="J31" s="7" t="s">
         <v>133</v>
@@ -4045,28 +4028,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="J32" s="16" t="s">
         <v>136</v>
@@ -4084,28 +4067,28 @@
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="J33" s="16" t="s">
         <v>139</v>
@@ -4123,28 +4106,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="J34" s="30" t="s">
         <v>142</v>
@@ -4162,28 +4145,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="J35" s="30" t="s">
         <v>144</v>
@@ -4201,28 +4184,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="J36" s="30" t="s">
         <v>147</v>
@@ -4240,28 +4223,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="J37" s="7" t="s">
         <v>150</v>
@@ -4279,28 +4262,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="J38" s="7" t="s">
         <v>153</v>
@@ -4318,28 +4301,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="J39" s="7" t="s">
         <v>156</v>
@@ -4386,16 +4369,16 @@
         <v>13</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="F1" s="23" t="s">
         <v>15</v>
@@ -4415,16 +4398,16 @@
         <v>101</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>19</v>
@@ -4444,16 +4427,16 @@
         <v>102</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>23</v>
@@ -4471,16 +4454,16 @@
         <v>103</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>26</v>
@@ -4496,16 +4479,16 @@
         <v>104</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>28</v>
@@ -4525,16 +4508,16 @@
         <v>105</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>32</v>
@@ -4552,16 +4535,16 @@
         <v>106</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>35</v>
@@ -4575,16 +4558,16 @@
         <v>107</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>36</v>
@@ -4600,16 +4583,16 @@
         <v>108</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>38</v>
@@ -4627,16 +4610,16 @@
         <v>109</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>41</v>
@@ -4650,16 +4633,16 @@
         <v>110</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>42</v>
@@ -4679,361 +4662,325 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.140625" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="21" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="34" t="s">
-        <v>498</v>
+      <c r="B2" s="33" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>536</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="33" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="B4" s="34" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="33" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="B5" s="34" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="33" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="B6" s="34" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="33" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" s="35" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="33" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="B9" s="35" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="33" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="B10" s="35" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="33" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="B11" s="35" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" s="33" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="B12" s="35" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" s="33" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="B13" s="35" t="s">
+    <row r="18" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="33" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="B14" s="35" t="s">
+    <row r="19" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="B23" s="33" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="B15" s="35" t="s">
+    <row r="24" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="B27" s="33" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="B16" s="35" t="s">
+    <row r="28" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="B28" s="33" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="B17" s="35" t="s">
+    <row r="29" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B34" s="33" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
-        <v>183</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="B22" s="36" t="s">
+    <row r="35" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="B37" s="33" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
-        <v>187</v>
-      </c>
-      <c r="B24" s="36" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="B25" s="36" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="B26" s="36" t="s">
+    <row r="38" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B38" s="33" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="27" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="B27" s="36" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="B28" s="36" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
-        <v>192</v>
-      </c>
-      <c r="B29" s="36" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
-        <v>193</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
-        <v>194</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
-        <v>196</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="B34" s="37" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="B35" s="32" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="B36" s="38" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="B37" s="38" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
-        <v>499</v>
-      </c>
-      <c r="B38" s="38" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
-        <v>499</v>
-      </c>
-      <c r="B39" s="38" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
-        <v>499</v>
-      </c>
-      <c r="B40" s="38" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
-        <v>499</v>
-      </c>
-      <c r="B41" s="38" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
-        <v>499</v>
-      </c>
-      <c r="B42" s="38" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
-        <v>499</v>
-      </c>
-      <c r="B43" s="38" t="s">
-        <v>536</v>
-      </c>
+    <row r="39" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1"/>
@@ -5047,7 +4994,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5068,7 +5015,7 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D1" t="s">
         <v>202</v>
@@ -5077,7 +5024,7 @@
         <v>203</v>
       </c>
       <c r="F1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -5085,7 +5032,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -5096,8 +5043,8 @@
       <c r="E2" t="s">
         <v>207</v>
       </c>
-      <c r="F2" t="s">
-        <v>210</v>
+      <c r="F2" s="33" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5105,7 +5052,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="C3">
         <v>14</v>
@@ -5116,8 +5063,8 @@
       <c r="E3" t="s">
         <v>208</v>
       </c>
-      <c r="F3" t="s">
-        <v>211</v>
+      <c r="F3" s="33" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5125,7 +5072,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -5136,8 +5083,8 @@
       <c r="E4" t="s">
         <v>209</v>
       </c>
-      <c r="F4" t="s">
-        <v>212</v>
+      <c r="F4" s="33" t="s">
+        <v>529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>